<commit_message>
import excel - russian names of columns
</commit_message>
<xml_diff>
--- a/_mat_tz/manures_for_import_eng__.xlsx
+++ b/_mat_tz/manures_for_import_eng__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_my_projects\manure\_mat_tz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA24616-7E40-42F9-87CF-3C52E7FAFF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66537768-C3E8-4FBA-85F0-047D7415AB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,34 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>norm_nitrogen</t>
-  </si>
-  <si>
-    <t>norm_phosphorus</t>
-  </si>
-  <si>
-    <t>norm_potassium</t>
-  </si>
-  <si>
-    <t>culture_id</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>purpose</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Район 1</t>
   </si>
@@ -88,7 +61,31 @@
     <t>имя2</t>
   </si>
   <si>
-    <t>вы</t>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Норма азота</t>
+  </si>
+  <si>
+    <t>Норма фосфора</t>
+  </si>
+  <si>
+    <t>Норма калия</t>
+  </si>
+  <si>
+    <t>Id культуры</t>
+  </si>
+  <si>
+    <t>Район</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Описание </t>
+  </si>
+  <si>
+    <t>Назначение</t>
   </si>
 </sst>
 </file>
@@ -412,45 +409,56 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
@@ -461,27 +469,27 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>123</v>
       </c>
       <c r="C3" s="1">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>222</v>
@@ -490,16 +498,16 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>